<commit_message>
true rankings altijd in permutations
</commit_message>
<xml_diff>
--- a/results/util-algo=mallows_costs-dist=betavariate_voters=200_projects=15/approved_voters.xlsx
+++ b/results/util-algo=mallows_costs-dist=betavariate_voters=200_projects=15/approved_voters.xlsx
@@ -1,37 +1,138 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>project0</t>
+  </si>
+  <si>
+    <t>project1</t>
+  </si>
+  <si>
+    <t>project2</t>
+  </si>
+  <si>
+    <t>project3</t>
+  </si>
+  <si>
+    <t>project4</t>
+  </si>
+  <si>
+    <t>project5</t>
+  </si>
+  <si>
+    <t>project6</t>
+  </si>
+  <si>
+    <t>project7</t>
+  </si>
+  <si>
+    <t>project8</t>
+  </si>
+  <si>
+    <t>project9</t>
+  </si>
+  <si>
+    <t>project10</t>
+  </si>
+  <si>
+    <t>project11</t>
+  </si>
+  <si>
+    <t>project12</t>
+  </si>
+  <si>
+    <t>project13</t>
+  </si>
+  <si>
+    <t>project14</t>
+  </si>
+  <si>
+    <t>approval</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>utility sum</t>
+  </si>
+  <si>
+    <t>utility ratio</t>
+  </si>
+  <si>
+    <t>utility product</t>
+  </si>
+  <si>
+    <t>cumulative sum</t>
+  </si>
+  <si>
+    <t>cumulative ratio</t>
+  </si>
+  <si>
+    <t>cumulative product</t>
+  </si>
+  <si>
+    <t>knapsack</t>
+  </si>
+  <si>
+    <t>knapsack ratio</t>
+  </si>
+  <si>
+    <t>default borda</t>
+  </si>
+  <si>
+    <t>default borda truncated</t>
+  </si>
+  <si>
+    <t>dowdall system borda</t>
+  </si>
+  <si>
+    <t>dowdall system borda truncated</t>
+  </si>
+  <si>
+    <t>eurovision song contest borda</t>
+  </si>
+  <si>
+    <t>eurovision song contest borda truncated</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +147,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -421,122 +463,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>project0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>project1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>project2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>project3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>project4</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>project5</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>project6</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>project7</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>project8</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>project9</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>project10</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>project11</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>project12</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>project13</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>project14</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>approval</t>
-        </is>
+    <row r="1" spans="1:16">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -548,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -560,17 +564,15 @@
         <v>0</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>threshold</t>
-        </is>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -585,10 +587,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -600,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -612,17 +614,15 @@
         <v>0</v>
       </c>
       <c r="P3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>utility sum</t>
-        </is>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -631,16 +631,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -667,11 +667,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>utility ratio</t>
-        </is>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -692,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -701,16 +699,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
       </c>
       <c r="N5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -719,14 +717,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>utility product</t>
-        </is>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -735,16 +731,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -771,14 +767,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>cumulative sum</t>
-        </is>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -787,16 +781,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -823,11 +817,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>cumulative ratio</t>
-        </is>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -848,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -857,16 +849,16 @@
         <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
       </c>
       <c r="N8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" t="b">
         <v>0</v>
@@ -875,14 +867,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>cumulative product</t>
-        </is>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -891,16 +881,16 @@
         <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -927,14 +917,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>knapsack</t>
-        </is>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -949,10 +937,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -964,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="L10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -976,14 +964,12 @@
         <v>0</v>
       </c>
       <c r="P10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>knapsack ratio</t>
-        </is>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -992,10 +978,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1019,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="M11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" t="b">
         <v>0</v>
@@ -1031,14 +1017,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>default borda</t>
-        </is>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1047,16 +1031,16 @@
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -1083,14 +1067,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>default borda truncated</t>
-        </is>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -1102,13 +1084,13 @@
         <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -1120,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1135,29 +1117,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>dowdall system borda</t>
-        </is>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -1172,13 +1152,13 @@
         <v>1</v>
       </c>
       <c r="L14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" t="b">
         <v>0</v>
@@ -1187,14 +1167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>dowdall system borda truncated</t>
-        </is>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1206,13 +1184,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -1224,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
@@ -1239,32 +1217,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>eurovision song contest borda</t>
-        </is>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -1276,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -1288,17 +1264,15 @@
         <v>0</v>
       </c>
       <c r="P16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>eurovision song contest borda truncated</t>
-        </is>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1310,13 +1284,13 @@
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -1328,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
@@ -1344,6 +1318,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>